<commit_message>
☑️ Feedback after mentor call
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nielsonderbeke/Desktop/3MCT-WAD/research-project/research-project-3mct/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nielsonderbeke/Desktop/3MCT-WAD/research-project/research-project-3mct-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CF5576-2B6C-7E4A-8359-A4167D573A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5BB875-D686-354D-81FC-9968088032ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34560" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetingen" sheetId="4" r:id="rId1"/>
@@ -392,11 +392,11 @@
     <xf numFmtId="164" fontId="2" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4326,24 +4326,24 @@
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28" t="s">
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28" t="s">
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
       <c r="N4" s="11"/>
       <c r="O4" s="11" t="s">
         <v>11</v>
@@ -4573,8 +4573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A49B06-8EDD-4703-89E7-71FF6DEBDE86}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5146,8 +5146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A5B55D-CB8B-7247-A828-793F51A9D090}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5199,20 +5199,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="172" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="28" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5220,14 +5220,14 @@
       <c r="A6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29" t="s">
+      <c r="C6" s="28"/>
+      <c r="D6" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="28" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5235,16 +5235,16 @@
       <c r="A7" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="28" t="s">
         <v>45</v>
       </c>
     </row>
@@ -5356,24 +5356,24 @@
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28" t="s">
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28" t="s">
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6" t="s">
         <v>11</v>

</xml_diff>